<commit_message>
update number of cities
</commit_message>
<xml_diff>
--- a/cities.xlsx
+++ b/cities.xlsx
@@ -5,7 +5,9 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$13</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
@@ -25,70 +27,70 @@
     <t>Area</t>
   </si>
   <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Pyeongchang</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Marakesh</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Albuquerque</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>Los Cabos</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Greenville</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Archipelago Sea</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Walla Walla Valley</t>
+  </si>
+  <si>
+    <t>Salina Island</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
     <t>Solta</t>
   </si>
   <si>
     <t>Croatia</t>
   </si>
   <si>
-    <t>Greenville</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Buenos Aires</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Los Cabos</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Walla Walla Valley</t>
-  </si>
-  <si>
-    <t>Marakesh</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Albuquerque</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>Archipelago Sea</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
     <t>Iguazu Falls</t>
-  </si>
-  <si>
-    <t>Salina Island</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Pyeongchang</t>
-  </si>
-  <si>
-    <t>South Korea</t>
   </si>
 </sst>
 </file>
@@ -204,10 +206,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>1700.0</v>
+        <v>2891000.0</v>
       </c>
       <c r="D2" s="2">
-        <v>59.0</v>
+        <v>4758.0</v>
       </c>
     </row>
     <row r="3">
@@ -218,10 +220,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>84554.0</v>
+        <v>2800000.0</v>
       </c>
       <c r="D3" s="2">
-        <v>68.0</v>
+        <v>2731571.0</v>
       </c>
     </row>
     <row r="4">
@@ -232,10 +234,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>1.3591863E7</v>
+        <v>2581000.0</v>
       </c>
       <c r="D4" s="2">
-        <v>4758.0</v>
+        <v>3194.0</v>
       </c>
     </row>
     <row r="5">
@@ -246,10 +248,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>287651.0</v>
+        <v>928850.0</v>
       </c>
       <c r="D5" s="2">
-        <v>3750.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="6">
@@ -257,49 +259,49 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>32237.0</v>
+        <v>559277.0</v>
       </c>
       <c r="D6" s="2">
-        <v>33.0</v>
+        <v>491.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>928850.0</v>
+        <v>287651.0</v>
       </c>
       <c r="D7" s="2">
-        <v>200.0</v>
+        <v>3750.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>559277.0</v>
+        <v>84554.0</v>
       </c>
       <c r="D8" s="2">
-        <v>491.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>60000.0</v>
@@ -310,24 +312,24 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>672.0</v>
+        <v>32237.0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>33.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>4000.0</v>
@@ -338,30 +340,30 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
-        <v>630.0</v>
+        <v>1700.0</v>
       </c>
       <c r="D12" s="2">
-        <v>2731571.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
-        <v>2581000.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3194.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>672.0</v>
       </c>
     </row>
     <row r="14">
@@ -407,6 +409,7 @@
       <c r="A31" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$D$13"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>